<commit_message>
Got courses showing up
</commit_message>
<xml_diff>
--- a/info/Data entry.xlsx
+++ b/info/Data entry.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Val\Desktop\GA project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Val\Desktop\ga-matcher\info\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A285939-C002-449D-931C-211FB71161F7}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{9FD0C80B-46E3-4E96-990E-13C1288AF9FB}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView minimized="1" xWindow="768" yWindow="768" windowWidth="17280" windowHeight="8964" xr2:uid="{A7331208-4913-47D9-98D5-AE3825B03CE4}"/>
   </bookViews>
@@ -18,6 +18,7 @@
     <sheet name="Sheet1" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -60,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="47">
   <si>
     <t>Class section</t>
   </si>
@@ -198,6 +199,9 @@
   </si>
   <si>
     <t xml:space="preserve">Professor Nominations </t>
+  </si>
+  <si>
+    <t>Hours</t>
   </si>
 </sst>
 </file>
@@ -281,19 +285,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -611,7 +611,7 @@
   <dimension ref="A1:L6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="103" zoomScaleNormal="70" workbookViewId="0">
-      <selection sqref="A1:M6"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -681,7 +681,7 @@
       <c r="D2">
         <v>35</v>
       </c>
-      <c r="E2" s="2">
+      <c r="E2">
         <f>ROUND(D2-1,-1)/2</f>
         <v>15</v>
       </c>
@@ -709,14 +709,14 @@
         <v>13</v>
       </c>
       <c r="C3" t="str">
-        <f t="shared" ref="C3:C6" si="0">B3&amp;" - "&amp;A3</f>
+        <f>B3&amp;" - "&amp;A3</f>
         <v>COMP 1900 - 2</v>
       </c>
       <c r="D3">
         <v>26</v>
       </c>
-      <c r="E3" s="2">
-        <f t="shared" ref="E3:E6" si="1">ROUND(D3-1,-1)/2</f>
+      <c r="E3">
+        <f>ROUND(D3-1,-1)/2</f>
         <v>15</v>
       </c>
       <c r="G3" t="s">
@@ -725,7 +725,7 @@
       <c r="I3">
         <v>2</v>
       </c>
-      <c r="J3" s="2" t="s">
+      <c r="J3" t="s">
         <v>39</v>
       </c>
     </row>
@@ -737,14 +737,14 @@
         <v>14</v>
       </c>
       <c r="C4" t="str">
-        <f t="shared" si="0"/>
+        <f>B4&amp;" - "&amp;A4</f>
         <v>COMP 4040 - 1</v>
       </c>
       <c r="D4">
         <v>40</v>
       </c>
-      <c r="E4" s="2">
-        <f t="shared" si="1"/>
+      <c r="E4">
+        <f>ROUND(D4-1,-1)/2</f>
         <v>20</v>
       </c>
       <c r="G4" t="s">
@@ -753,7 +753,7 @@
       <c r="I4">
         <v>2</v>
       </c>
-      <c r="J4" s="2" t="s">
+      <c r="J4" t="s">
         <v>39</v>
       </c>
     </row>
@@ -764,15 +764,15 @@
       <c r="B5" t="s">
         <v>41</v>
       </c>
-      <c r="C5" s="2" t="str">
-        <f t="shared" si="0"/>
+      <c r="C5" t="str">
+        <f>B5&amp;" - "&amp;A5</f>
         <v>COMP 6300 - 1</v>
       </c>
       <c r="D5">
         <v>26</v>
       </c>
-      <c r="E5" s="2">
-        <f t="shared" si="1"/>
+      <c r="E5">
+        <f>ROUND(D5-1,-1)/2</f>
         <v>15</v>
       </c>
       <c r="I5">
@@ -789,15 +789,15 @@
       <c r="B6" t="s">
         <v>42</v>
       </c>
-      <c r="C6" s="2" t="str">
-        <f t="shared" si="0"/>
+      <c r="C6" t="str">
+        <f>B6&amp;" - "&amp;A6</f>
         <v>COMP 6400 - 1</v>
       </c>
       <c r="D6">
         <v>16</v>
       </c>
-      <c r="E6" s="2">
-        <f t="shared" si="1"/>
+      <c r="E6">
+        <f>ROUND(D6-1,-1)/2</f>
         <v>10</v>
       </c>
       <c r="I6">
@@ -815,10 +815,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D7B39D2-6E79-4819-8F36-7B1ACE07D65B}">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D20" activeCellId="1" sqref="A1 D20"/>
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -831,7 +831,7 @@
     <col min="6" max="6" width="13.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" s="1" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
@@ -850,89 +850,110 @@
       <c r="F1" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A2" s="5" t="s">
+      <c r="G1" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="C2" s="5" t="s">
         <v>20</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" s="5" t="s">
+      <c r="G2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="3" t="s">
         <v>23</v>
       </c>
       <c r="E3" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" s="3" t="s">
+      <c r="G3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="3" t="s">
         <v>26</v>
       </c>
       <c r="E4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" s="3" t="s">
+      <c r="G4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="3" t="s">
         <v>29</v>
       </c>
       <c r="E5" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" s="7" t="s">
+      <c r="G5">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="3" t="s">
         <v>32</v>
       </c>
       <c r="E6" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7" s="5" t="s">
+      <c r="G6">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C7" s="4" t="s">
         <v>35</v>
       </c>
       <c r="E7" t="s">
         <v>17</v>
+      </c>
+      <c r="G7">
+        <v>400</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Put Names and Courses on the home page
</commit_message>
<xml_diff>
--- a/info/Data entry.xlsx
+++ b/info/Data entry.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Val\Desktop\ga-matcher\info\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9FD0C80B-46E3-4E96-990E-13C1288AF9FB}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FE7913C-3DA1-4D4D-ACFB-EA2F25EBBF5F}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="768" yWindow="768" windowWidth="17280" windowHeight="8964" xr2:uid="{A7331208-4913-47D9-98D5-AE3825B03CE4}"/>
+    <workbookView xWindow="384" yWindow="384" windowWidth="17280" windowHeight="8964" xr2:uid="{A7331208-4913-47D9-98D5-AE3825B03CE4}"/>
   </bookViews>
   <sheets>
     <sheet name="Classes" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,6 @@
     <sheet name="Sheet1" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -61,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="48">
   <si>
     <t>Class section</t>
   </si>
@@ -72,9 +71,6 @@
     <t>Current Enrollment</t>
   </si>
   <si>
-    <t>Credit hours needed</t>
-  </si>
-  <si>
     <t>Time slots</t>
   </si>
   <si>
@@ -96,9 +92,6 @@
     <t>Attendance preferred?</t>
   </si>
   <si>
-    <t>GA nomination</t>
-  </si>
-  <si>
     <t>Instructor priority</t>
   </si>
   <si>
@@ -202,6 +195,15 @@
   </si>
   <si>
     <t>Hours</t>
+  </si>
+  <si>
+    <t>GA hours needed</t>
+  </si>
+  <si>
+    <t>Full Department</t>
+  </si>
+  <si>
+    <t>Sen</t>
   </si>
 </sst>
 </file>
@@ -608,10 +610,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{562170CF-388F-4544-8E9F-61CB35D9D9B0}">
-  <dimension ref="A1:L6"/>
+  <dimension ref="A1:J7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="103" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="103" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -629,7 +631,7 @@
     <col min="12" max="12" width="10.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -637,42 +639,36 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D1" t="s">
         <v>2</v>
       </c>
       <c r="E1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
-        <v>4</v>
-      </c>
       <c r="G1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" t="s">
         <v>9</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>10</v>
       </c>
-      <c r="I1" t="s">
-        <v>12</v>
-      </c>
       <c r="J1" t="s">
-        <v>38</v>
-      </c>
-      <c r="K1" t="s">
-        <v>44</v>
-      </c>
-      <c r="L1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C2" t="str">
         <f>B2&amp;" - "&amp;A2</f>
@@ -686,27 +682,27 @@
         <v>15</v>
       </c>
       <c r="F2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="G2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="H2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="I2">
         <v>2</v>
       </c>
       <c r="J2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C3" t="str">
         <f>B3&amp;" - "&amp;A3</f>
@@ -720,21 +716,21 @@
         <v>15</v>
       </c>
       <c r="G3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="I3">
         <v>2</v>
       </c>
       <c r="J3" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C4" t="str">
         <f>B4&amp;" - "&amp;A4</f>
@@ -748,21 +744,21 @@
         <v>20</v>
       </c>
       <c r="G4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="I4">
         <v>2</v>
       </c>
       <c r="J4" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C5" t="str">
         <f>B5&amp;" - "&amp;A5</f>
@@ -779,15 +775,15 @@
         <v>3</v>
       </c>
       <c r="J5" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>1</v>
       </c>
       <c r="B6" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C6" t="str">
         <f>B6&amp;" - "&amp;A6</f>
@@ -804,7 +800,12 @@
         <v>1</v>
       </c>
       <c r="J6" t="s">
-        <v>40</v>
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B7" t="s">
+        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -815,10 +816,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D7B39D2-6E79-4819-8F36-7B1ACE07D65B}">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -828,131 +829,137 @@
     <col min="3" max="3" width="10.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18.44140625" customWidth="1"/>
     <col min="5" max="5" width="15.88671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.21875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" s="1" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>8</v>
-      </c>
       <c r="F1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+        <v>44</v>
+      </c>
+      <c r="G1" t="s">
+        <v>42</v>
+      </c>
+      <c r="H1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="D2" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F2">
+        <v>5</v>
+      </c>
+      <c r="H2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="B3" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="G2">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
+      <c r="C3" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="E3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="B4" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="E3" t="s">
-        <v>17</v>
-      </c>
-      <c r="G3">
+      <c r="C4" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B4" s="2" t="s">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="B5" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="E4" t="s">
-        <v>17</v>
-      </c>
-      <c r="G4">
+      <c r="C5" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F5">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E6" t="s">
+        <v>15</v>
+      </c>
+      <c r="F6">
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="E5" t="s">
-        <v>17</v>
-      </c>
-      <c r="G5">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B6" s="2" t="s">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="B7" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="E6" t="s">
-        <v>17</v>
-      </c>
-      <c r="G6">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" s="2" t="s">
+      <c r="C7" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="B7" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>35</v>
-      </c>
       <c r="E7" t="s">
-        <v>17</v>
-      </c>
-      <c r="G7">
+        <v>15</v>
+      </c>
+      <c r="F7">
         <v>400</v>
       </c>
     </row>

</xml_diff>